<commit_message>
feat: :sparkles: Filtragem de Elementos por Tipos
</commit_message>
<xml_diff>
--- a/meuarquivo.xlsx
+++ b/meuarquivo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Identificacao do Documento</t>
   </si>
@@ -43,34 +43,115 @@
     <t>Prazo para Entrega</t>
   </si>
   <si>
+    <t>Empréstimo</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>2024-05-18</t>
+  </si>
+  <si>
+    <t>credito</t>
+  </si>
+  <si>
+    <t>12.000</t>
+  </si>
+  <si>
+    <t>pendente</t>
+  </si>
+  <si>
+    <t>Higor</t>
+  </si>
+  <si>
+    <t>documento .... ....</t>
+  </si>
+  <si>
+    <t>2024-07-18</t>
+  </si>
+  <si>
     <t>Empréstimo Consignado</t>
   </si>
   <si>
-    <t>Alexandre Junior Pereira Gomes Hernandes</t>
-  </si>
-  <si>
-    <t>2024-05-18</t>
-  </si>
-  <si>
-    <t>12999</t>
-  </si>
-  <si>
-    <t>pendente</t>
-  </si>
-  <si>
-    <t>2024-06-06</t>
-  </si>
-  <si>
-    <t>Doação para caridade</t>
-  </si>
-  <si>
-    <t>Governo Brasileiro</t>
-  </si>
-  <si>
-    <t>2024-05-23</t>
-  </si>
-  <si>
-    <t>credito</t>
+    <t>Ednaldo Pereira Gomes</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>Higor Vital Lopo</t>
+  </si>
+  <si>
+    <t>investimento consignado institucional paralelo ao indiana jones</t>
+  </si>
+  <si>
+    <t>2024-06-14</t>
+  </si>
+  <si>
+    <t>Doação Monetária</t>
+  </si>
+  <si>
+    <t>Davy Jones Da Silva</t>
+  </si>
+  <si>
+    <t>2024-05-17</t>
+  </si>
+  <si>
+    <t>debito</t>
+  </si>
+  <si>
+    <t>99999999</t>
+  </si>
+  <si>
+    <t>Higor Vital</t>
+  </si>
+  <si>
+    <t>muito dinheiro envolvido.</t>
+  </si>
+  <si>
+    <t>Empréstimo Bancário Rico Emprestoso Valioso Institucional</t>
+  </si>
+  <si>
+    <t>Eduardo Hernandes Cunha Ferreira Da Silva Castro</t>
+  </si>
+  <si>
+    <t>1200000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higor Vital Lopo </t>
+  </si>
+  <si>
+    <t>Este é um documento institucional raro caro para o Loren Ipsum Dolor Ammet Caract Errani Dragon Ball Budokai Tenkaishi 3</t>
+  </si>
+  <si>
+    <t>2024-06-07</t>
+  </si>
+  <si>
+    <t>Emprestimo futuro</t>
+  </si>
+  <si>
+    <t>Futurama</t>
+  </si>
+  <si>
+    <t>2024-06-08</t>
+  </si>
+  <si>
+    <t>andamento</t>
+  </si>
+  <si>
+    <t>eu do futuro</t>
+  </si>
+  <si>
+    <t>futuro</t>
+  </si>
+  <si>
+    <t>2024-07-05</t>
+  </si>
+  <si>
+    <t>emprestimo</t>
+  </si>
+  <si>
+    <t>higor</t>
   </si>
   <si>
     <t>99999</t>
@@ -79,139 +160,22 @@
     <t>concluido</t>
   </si>
   <si>
-    <t>Higor Vital Lopo</t>
-  </si>
-  <si>
-    <t>emprestimo realizado sob encargo juridico para resolver problemas ambientais.</t>
-  </si>
-  <si>
-    <t>2024-06-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teste </t>
-  </si>
-  <si>
-    <t>eduardo</t>
-  </si>
-  <si>
-    <t>2024-05-17</t>
-  </si>
-  <si>
-    <t>debito</t>
-  </si>
-  <si>
-    <t>120000</t>
-  </si>
-  <si>
-    <t>higor vital lopo</t>
-  </si>
-  <si>
-    <t>aoinor wonoiwi woirnwioin</t>
-  </si>
-  <si>
-    <t>undefined/undefined/2024-06-13</t>
-  </si>
-  <si>
-    <t>Documentação Teste Erradicacional</t>
-  </si>
-  <si>
-    <t>Paralelepipedo Erosterides</t>
-  </si>
-  <si>
-    <t>9999</t>
-  </si>
-  <si>
-    <t>Elizanderes Calimondres</t>
-  </si>
-  <si>
-    <t>alknojs oaijaij oqineoiq qiqnoin</t>
-  </si>
-  <si>
-    <t>19/6/2024</t>
-  </si>
-  <si>
-    <t>Empréstimo Consignado Absurdo Para o Presidente dos Estados Unidos Da America</t>
-  </si>
-  <si>
-    <t>Joe Biden</t>
-  </si>
-  <si>
-    <t>9999999</t>
-  </si>
-  <si>
-    <t>andamento</t>
-  </si>
-  <si>
-    <t>emporetnoina loren ipsum dollor ammet sidrat</t>
-  </si>
-  <si>
-    <t>2024-07-11</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>209390</t>
-  </si>
-  <si>
-    <t>2024-06-13</t>
-  </si>
-  <si>
-    <t>TESTE</t>
-  </si>
-  <si>
-    <t>TESTE TESTADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMPRESTIMO ALIENIGENA </t>
-  </si>
-  <si>
-    <t>EIRUAO</t>
-  </si>
-  <si>
-    <t>90038298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aoinioa aiunon qoiniqono </t>
-  </si>
-  <si>
-    <t>documento institucional paralelepipedo</t>
-  </si>
-  <si>
-    <t>Alemao</t>
-  </si>
-  <si>
-    <t>12990180</t>
-  </si>
-  <si>
-    <t>ksjaon unoiqeinon</t>
-  </si>
-  <si>
-    <t>2024-06-15</t>
-  </si>
-  <si>
-    <t>ROUBO</t>
-  </si>
-  <si>
-    <t>OZIMANDIAS</t>
-  </si>
-  <si>
-    <t>098189318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexandre o grande </t>
-  </si>
-  <si>
-    <t>0svono aoin oainen aoinoin</t>
-  </si>
-  <si>
-    <t>AGORA</t>
-  </si>
-  <si>
-    <t>2024-05-16</t>
-  </si>
-  <si>
-    <t>10929019</t>
+    <t>jfonion</t>
+  </si>
+  <si>
+    <t>2024-05-31</t>
+  </si>
+  <si>
+    <t>Declaração de Imposto de Renda</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Higor V.L.</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -537,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -594,34 +558,43 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -650,7 +623,7 @@
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -659,59 +632,59 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>36</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -722,205 +695,60 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: :sparkles: Busca e Interação por ID
</commit_message>
<xml_diff>
--- a/meuarquivo.xlsx
+++ b/meuarquivo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Plan1" state="visible" r:id="rId4"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Identificação do Documento</t>
   </si>
@@ -41,6 +41,57 @@
   </si>
   <si>
     <t>Prazo para Entrega</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
+    <t>debito</t>
+  </si>
+  <si>
+    <t>pendente</t>
+  </si>
+  <si>
+    <t>2024-06-06</t>
+  </si>
+  <si>
+    <t>19f0461e-77e6-4fda-89c0-5272cfa5cd1e</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2024-06-01</t>
+  </si>
+  <si>
+    <t>9bc64b2a-58d5-460f-a221-10be768ac18f</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2024-05-24</t>
+  </si>
+  <si>
+    <t>credito</t>
+  </si>
+  <si>
+    <t>4bc00f54-2428-4342-9c5b-9ec7e10ceefa</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2024-05-31</t>
+  </si>
+  <si>
+    <t>016b8ba6-86db-4d78-94b8-07c086f7f2d2</t>
   </si>
 </sst>
 </file>
@@ -358,26 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,10 +444,140 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>